<commit_message>
Email verifier synchronus done.
</commit_message>
<xml_diff>
--- a/src/test/resource/EmailList.xlsx
+++ b/src/test/resource/EmailList.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Email Address</t>
   </si>
@@ -33,20 +33,34 @@
     <t>zztop_aditya2@yahoo.com</t>
   </si>
   <si>
-    <t>test123</t>
+    <t>eldrid.aditya@mail.rakuten.com</t>
+  </si>
+  <si>
+    <t>yue_nix@yahoo.com</t>
+  </si>
+  <si>
+    <t>yue_nix2@yahoo.com</t>
+  </si>
+  <si>
+    <t>ninik.yang@gmail.com</t>
+  </si>
+  <si>
+    <t>eldrid_a1@verifone.com</t>
+  </si>
+  <si>
+    <t>e.aditya@netbiscuits.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -56,6 +70,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -76,15 +98,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -415,75 +443,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+    </row>
+    <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+    </row>
+    <row r="4" spans="1:1">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:2">
+    <row r="5" spans="1:1">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
       <c r="A7" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
       <c r="A8" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
       <c r="A9" s="1" t="s">
-        <v>1</v>
-      </c>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A6" r:id="rId4"/>
-    <hyperlink ref="A7" r:id="rId5"/>
-    <hyperlink ref="A8" r:id="rId6"/>
-    <hyperlink ref="A9" r:id="rId7"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
+    <hyperlink ref="A9" r:id="rId8"/>
+    <hyperlink ref="A10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Subscriber Management added and changes in entity.
</commit_message>
<xml_diff>
--- a/src/test/resource/EmailList.xlsx
+++ b/src/test/resource/EmailList.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Email Address</t>
   </si>
@@ -36,19 +36,10 @@
     <t>eldrid.aditya@mail.rakuten.com</t>
   </si>
   <si>
-    <t>yue_nix@yahoo.com</t>
-  </si>
-  <si>
-    <t>yue_nix2@yahoo.com</t>
-  </si>
-  <si>
-    <t>ninik.yang@gmail.com</t>
-  </si>
-  <si>
-    <t>eldrid_a1@verifone.com</t>
-  </si>
-  <si>
     <t>e.aditya@netbiscuits.com</t>
+  </si>
+  <si>
+    <t>equivipte@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -443,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -481,31 +472,16 @@
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="1"/>
+      <c r="A8" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -515,9 +491,6 @@
     <hyperlink ref="A5" r:id="rId4"/>
     <hyperlink ref="A6" r:id="rId5"/>
     <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
-    <hyperlink ref="A9" r:id="rId8"/>
-    <hyperlink ref="A10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Modify Subscriber Entity and Subcriber management screen
</commit_message>
<xml_diff>
--- a/src/test/resource/EmailList.xlsx
+++ b/src/test/resource/EmailList.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Email Address</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>equivipte@gmail.com</t>
+  </si>
+  <si>
+    <t>x2@mail.rakuten.com</t>
+  </si>
+  <si>
+    <t>equivipte2@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -89,9 +95,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -100,10 +108,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -434,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -481,7 +491,14 @@
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -491,6 +508,8 @@
     <hyperlink ref="A5" r:id="rId4"/>
     <hyperlink ref="A6" r:id="rId5"/>
     <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
+    <hyperlink ref="A9" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>